<commit_message>
adding weight data for NS4, NS5, and NS6
</commit_message>
<xml_diff>
--- a/Data/Weight_data.xlsx
+++ b/Data/Weight_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Nonlinearity\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E269F5CB-FF84-4A1E-9AB0-0DFA29EE30D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD689DDD-2D88-4F84-AD55-CCC53C800478}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D48B6DC4-DE78-402F-9666-E065354627DD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="27">
   <si>
     <t>Sample Number</t>
   </si>
@@ -76,13 +76,52 @@
   </si>
   <si>
     <t>Fracture</t>
+  </si>
+  <si>
+    <t>NS4</t>
+  </si>
+  <si>
+    <t>NS5</t>
+  </si>
+  <si>
+    <t>Sample: NS1</t>
+  </si>
+  <si>
+    <t>Conditon</t>
+  </si>
+  <si>
+    <t>Water infiltrated</t>
+  </si>
+  <si>
+    <t>Weight (g)</t>
+  </si>
+  <si>
+    <t>Water removed</t>
+  </si>
+  <si>
+    <t>Sample: NS2</t>
+  </si>
+  <si>
+    <t>Sample: NS3</t>
+  </si>
+  <si>
+    <t>Sample: NS4</t>
+  </si>
+  <si>
+    <t>Sample: NS5</t>
+  </si>
+  <si>
+    <t>Sample: NS6</t>
+  </si>
+  <si>
+    <t>NS6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,16 +129,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -107,12 +172,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,173 +513,964 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337C877C-E8A4-4517-AE8C-A94108AF12C7}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
         <v>1199.4000000000001</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1199.4000000000001</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1189.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3">
         <v>1255.0999999999999</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1255.0999999999999</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1252.4000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4">
         <v>1187.3</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1187.3</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1187.4000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3">
         <v>1292.5999999999999</v>
       </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="1">
+        <f>I3-I2</f>
+        <v>55.699999999999818</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="1">
+        <f>M3-M2</f>
+        <v>63.200000000000045</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1216.2</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="1">
+        <f>I3-I4</f>
+        <v>67.799999999999955</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="1">
+        <f>M3-M4</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1233.5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1295.3</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1195.4000000000001</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="K9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1225.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>1216.2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1189.2</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1292.5999999999999</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1283.9000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1225.7</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1216.0999999999999</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1252.4000000000001</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" s="1">
+        <f>M10-M9</f>
+        <v>58.200000000000045</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1187.4000000000001</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="1">
+        <f>I10-I11</f>
+        <v>76.5</v>
+      </c>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="1">
+        <f>M10-M11</f>
+        <v>67.900000000000091</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1253.5999999999999</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1222.4000000000001</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1283.9000000000001</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="1">
         <v>1233.5</v>
       </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="K16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1229.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1247.7</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1295.3</v>
+      </c>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M17" s="1">
+        <v>1285.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1190.8</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1222.4000000000001</v>
+      </c>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1221.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1322.4</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="1">
+        <f>I17-I16</f>
+        <v>61.799999999999955</v>
+      </c>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M19" s="1">
+        <f>M17-M16</f>
+        <v>56.299999999999955</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1216</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="1">
+        <f>I17-I18</f>
+        <v>72.899999999999864</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" s="1">
+        <f>M17-M18</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>1295.3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <v>1195.4000000000001</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10">
-        <v>1189.2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <v>1252.3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
+      <c r="B21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1229.5</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1243.3</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1285.8</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1195.3</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M23" s="1">
+        <v>1193.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1193.7</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="1">
+        <v>1253.5999999999999</v>
+      </c>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M24" s="1">
+        <v>1253.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="4">
+        <v>1221.8</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1190.8</v>
+      </c>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M25" s="1">
+        <v>1190.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1253.7</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26" s="1">
+        <f>I24-I23</f>
+        <v>58.299999999999955</v>
+      </c>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M26" s="1">
+        <f>M24-M23</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="4">
+        <v>1190.7</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I27" s="1">
+        <f>I24-I25</f>
+        <v>62.799999999999955</v>
+      </c>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M27" s="1">
+        <f>M24-M25</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1202.0999999999999</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1270.2</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I30" s="1">
+        <v>1247.7</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G31" s="1"/>
+      <c r="H31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="1">
+        <v>1322.4</v>
+      </c>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M31" s="1"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G32" s="1"/>
+      <c r="H32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I32" s="1">
+        <v>1243.3</v>
+      </c>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M32" s="1"/>
+    </row>
+    <row r="33" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G33" s="1"/>
+      <c r="H33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33" s="1">
+        <f>I31-I30</f>
+        <v>74.700000000000045</v>
+      </c>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M33" s="1"/>
+    </row>
+    <row r="34" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G34" s="1"/>
+      <c r="H34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I34" s="1">
+        <f>I31-I32</f>
+        <v>79.100000000000136</v>
+      </c>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M34" s="1"/>
+    </row>
+    <row r="36" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I37" s="6">
+        <v>1202.0999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G38" s="1"/>
+      <c r="H38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I38" s="1">
+        <v>1270.2</v>
+      </c>
+    </row>
+    <row r="39" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G39" s="1"/>
+      <c r="H39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G40" s="1"/>
+      <c r="H40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" s="1">
+        <f>I38-I37</f>
+        <v>68.100000000000136</v>
+      </c>
+    </row>
+    <row r="41" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G41" s="1"/>
+      <c r="H41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I41" s="1">
+        <f>I38-I39</f>
+        <v>1270.2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding NS6 initial weights and NS5 fracture weights
</commit_message>
<xml_diff>
--- a/Data/Weight_data.xlsx
+++ b/Data/Weight_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Nonlinearity\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD689DDD-2D88-4F84-AD55-CCC53C800478}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71088FC9-5A21-480B-A675-96CC0B356E02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D48B6DC4-DE78-402F-9666-E065354627DD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="27">
   <si>
     <t>Sample Number</t>
   </si>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337C877C-E8A4-4517-AE8C-A94108AF12C7}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1336,6 +1336,18 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="4">
+        <v>1198.4000000000001</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="G30" s="1" t="s">
         <v>5</v>
       </c>
@@ -1351,9 +1363,23 @@
       <c r="L30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M30" s="1"/>
+      <c r="M30" s="1">
+        <v>1247.0999999999999</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1247.0999999999999</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1" t="s">
         <v>7</v>
@@ -1365,9 +1391,23 @@
       <c r="L31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M31" s="1"/>
+      <c r="M31" s="1">
+        <v>1309.8</v>
+      </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1309.9000000000001</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
         <v>8</v>
@@ -1379,9 +1419,23 @@
       <c r="L32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M32" s="1"/>
-    </row>
-    <row r="33" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="M32" s="1">
+        <v>1243.4000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="4">
+        <v>1243.4000000000001</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1" t="s">
         <v>18</v>
@@ -1394,9 +1448,12 @@
       <c r="L33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M33" s="1"/>
-    </row>
-    <row r="34" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="M33" s="1">
+        <f>M31-M30</f>
+        <v>62.700000000000045</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G34" s="1"/>
       <c r="H34" s="1" t="s">
         <v>20</v>
@@ -1409,9 +1466,12 @@
       <c r="L34" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M34" s="1"/>
-    </row>
-    <row r="36" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="M34" s="1">
+        <f>M31-M32</f>
+        <v>66.399999999999864</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G36" s="1" t="s">
         <v>25</v>
       </c>
@@ -1422,7 +1482,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G37" s="1" t="s">
         <v>5</v>
       </c>
@@ -1433,7 +1493,7 @@
         <v>1202.0999999999999</v>
       </c>
     </row>
-    <row r="38" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G38" s="1"/>
       <c r="H38" s="1" t="s">
         <v>7</v>
@@ -1442,14 +1502,16 @@
         <v>1270.2</v>
       </c>
     </row>
-    <row r="39" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G39" s="1"/>
       <c r="H39" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="I39" s="1">
+        <v>1198.4000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G40" s="1"/>
       <c r="H40" s="1" t="s">
         <v>18</v>
@@ -1459,14 +1521,14 @@
         <v>68.100000000000136</v>
       </c>
     </row>
-    <row r="41" spans="7:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G41" s="1"/>
       <c r="H41" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I41" s="1">
         <f>I38-I39</f>
-        <v>1270.2</v>
+        <v>71.799999999999955</v>
       </c>
     </row>
   </sheetData>

</xml_diff>